<commit_message>
created a simplification so i can foucs on analysis on WSM which can then be generalized
</commit_message>
<xml_diff>
--- a/quarterly&annual_results/WSM_Modeling.xlsx
+++ b/quarterly&annual_results/WSM_Modeling.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/russell/Documents/Code/Python/Videos/Edgar_API_Video/quarterly&amp;annual_results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47F14C00-D96D-F847-AFDF-458434DF65A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBF21C4E-5920-CA40-B821-B8EB5F0E190B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="1" xr2:uid="{EFB7F790-841D-A948-97C7-C87C4CE19F81}"/>
+    <workbookView xWindow="-38400" yWindow="680" windowWidth="38400" windowHeight="21600" xr2:uid="{EFB7F790-841D-A948-97C7-C87C4CE19F81}"/>
   </bookViews>
   <sheets>
     <sheet name="Balance_Sheets" sheetId="1" r:id="rId1"/>
     <sheet name="Income_Statements" sheetId="2" r:id="rId2"/>
     <sheet name="Cash_Flow_Statements" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -574,7 +574,17 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -907,11 +917,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E6BBCCD-2EAE-E74A-BE70-7F1DB1770C28}">
   <dimension ref="A1:BC106"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B51" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F39" sqref="F39"/>
+      <selection pane="bottomRight" activeCell="E76" sqref="E76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7955,11 +7965,11 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="A57:N106">
+    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
+  </conditionalFormatting>
   <conditionalFormatting sqref="B1:BC52">
     <cfRule type="duplicateValues" dxfId="1" priority="2"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A57:N106">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7969,11 +7979,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CB6F779-C751-1E4D-B848-11E4653AC503}">
   <dimension ref="A1:AR47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C51" sqref="C51"/>
+      <selection pane="bottomRight" activeCell="AR8" sqref="AR8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10845,10 +10855,10 @@
   <dimension ref="A1:AP152"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B65" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B75" sqref="B75"/>
+      <selection pane="bottomRight" activeCell="A105" sqref="A105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -17634,6 +17644,10 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="B76:O152">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>